<commit_message>
Added LAFC to team name links
</commit_message>
<xml_diff>
--- a/TeamNameLinks.xlsx
+++ b/TeamNameLinks.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthias.Kullowatz\Documents\GitHub\ASAShootingApp_master\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="36" windowWidth="20112" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="54">
   <si>
     <t>L.A. Galaxy</t>
   </si>
@@ -172,13 +177,19 @@
   </si>
   <si>
     <t>NE</t>
+  </si>
+  <si>
+    <t>LAFC</t>
+  </si>
+  <si>
+    <t>Los Angeles FC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +226,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -261,7 +280,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -293,9 +312,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -327,6 +347,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -502,19 +523,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -522,7 +543,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -530,7 +551,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -538,7 +559,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -546,7 +567,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -554,7 +575,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -562,7 +583,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -570,7 +591,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -578,7 +599,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -586,7 +607,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -594,7 +615,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -602,7 +623,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -610,7 +631,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -618,7 +639,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -626,7 +647,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -634,7 +655,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -642,7 +663,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -650,7 +671,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -658,7 +679,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -666,7 +687,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -674,7 +695,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -682,7 +703,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -690,7 +711,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -698,7 +719,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -709,7 +730,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -720,7 +741,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -731,7 +752,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -742,7 +763,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -753,7 +774,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -764,7 +785,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -775,7 +796,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -786,7 +807,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -797,7 +818,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -808,7 +829,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -819,7 +840,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -830,7 +851,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -838,7 +859,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -849,7 +870,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -860,7 +881,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -871,7 +892,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -882,7 +903,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -893,12 +914,28 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>26</v>
       </c>
       <c r="B42" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -907,24 +944,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>